<commit_message>
new results for loc & resources
</commit_message>
<xml_diff>
--- a/results/2013.08.30_heston_sl_laptop/results_laptop.xlsx
+++ b/results/2013.08.30_heston_sl_laptop/results_laptop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="8610" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,10 +109,11 @@
     <t>Performance (run_cpu):</t>
   </si>
   <si>
-    <t>Display aus, Batterie raus, Netwerk aus, Wifi aus, Reboot &amp; Warmup, Multiple starts</t>
-  </si>
-  <si>
     <t>Flags: /O2 /arch:AVX /fp:fast /GL</t>
+  </si>
+  <si>
+    <t>Display aus, Batterie raus, Netwerk aus, Wifi aus, 
+Reboot &amp; Warmup, Multiple starts</t>
   </si>
 </sst>
 </file>
@@ -171,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -183,6 +184,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="48" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -487,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +542,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -637,7 +644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <f>A29/A26</f>
         <v>2.5467745638200184E-7</v>
@@ -646,17 +653,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>141086000</v>
       </c>
@@ -664,12 +671,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -677,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -685,7 +692,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -693,26 +700,31 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C44">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9">
         <v>30.6</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <f>C44/A38</f>
         <v>2.1688898969422907E-7</v>
@@ -722,7 +734,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E44:I44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>